<commit_message>
one coop tech dep 12 - fix spelling of cooptech
</commit_message>
<xml_diff>
--- a/db/uploads/cooptech.xlsx
+++ b/db/uploads/cooptech.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ansellgabrieldelayre/Sites/GA_system/db/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDF0E48-E79E-CE45-B816-A80DEA7DD41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6C80AC-24C8-FC4E-8BAA-72EB69FD66FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="2060" windowWidth="27240" windowHeight="16440" xr2:uid="{78331180-7D44-384E-90CD-6A6B98219BBB}"/>
+    <workbookView xWindow="3000" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{78331180-7D44-384E-90CD-6A6B98219BBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1265,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810354AC-C795-7A42-9E36-5E84AA0B018D}">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3279,5 +3279,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>